<commit_message>
adjusting more handouts for chapter 2
</commit_message>
<xml_diff>
--- a/handouts/chapter_2_1_handout.xlsx
+++ b/handouts/chapter_2_1_handout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RData\BYUI-Timeseries-Drafts\handouts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RussellStuff\Time series personal work\timeseries\handouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{085EEA26-1A85-46A9-BD3C-D1656D4CDEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DCA778-F97C-445F-A7DE-265658DEFE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB73943A-C465-40BE-817C-B9991112161C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{CB73943A-C465-40BE-817C-B9991112161C}"/>
   </bookViews>
   <sheets>
     <sheet name="Workbook" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>A14*A15*A16 Should be equal to this value</t>
         </r>
@@ -119,10 +119,10 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,8 +135,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -244,21 +250,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="1"/>
       </left>
       <right style="thin">
@@ -289,21 +280,6 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="1"/>
       </left>
       <right style="thin">
@@ -321,19 +297,6 @@
       </left>
       <right style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -417,11 +380,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -439,26 +465,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -468,19 +500,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -565,8 +600,8 @@
       <xdr:rowOff>45593</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="196079" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -648,7 +683,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -823,8 +858,8 @@
       <xdr:rowOff>45593</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="197298" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -906,7 +941,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -971,8 +1006,8 @@
       <xdr:rowOff>60833</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="510973" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="TextBox 16">
@@ -1078,7 +1113,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="TextBox 16">
@@ -1143,8 +1178,8 @@
       <xdr:rowOff>53213</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="663515" cy="225446"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="TextBox 17">
@@ -1281,7 +1316,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="TextBox 17">
@@ -1346,8 +1381,8 @@
       <xdr:rowOff>53213</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="514756" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="19" name="TextBox 18">
@@ -1453,7 +1488,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="19" name="TextBox 18">
@@ -1518,8 +1553,8 @@
       <xdr:rowOff>68453</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="667299" cy="225446"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="TextBox 19">
@@ -1656,7 +1691,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="TextBox 19">
@@ -1721,8 +1756,8 @@
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1210395" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="TextBox 20">
@@ -1895,7 +1930,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="TextBox 20">
@@ -1960,8 +1995,8 @@
       <xdr:rowOff>68453</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="134588" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="TextBox 22">
@@ -2036,7 +2071,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="23" name="TextBox 22">
@@ -2101,8 +2136,8 @@
       <xdr:rowOff>60833</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="137153" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="TextBox 23">
@@ -2177,7 +2212,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="TextBox 23">
@@ -2242,8 +2277,8 @@
       <xdr:rowOff>60833</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="197042" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="TextBox 24">
@@ -2325,7 +2360,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="TextBox 24">
@@ -2390,8 +2425,8 @@
       <xdr:rowOff>45593</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="202235" cy="232436"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="29" name="TextBox 28">
@@ -2473,7 +2508,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="29" name="TextBox 28">
@@ -2538,8 +2573,8 @@
       <xdr:rowOff>68453</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="122982" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="30" name="TextBox 29">
@@ -2602,7 +2637,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="30" name="TextBox 29">
@@ -2667,8 +2702,8 @@
       <xdr:rowOff>68453</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="735073" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="32" name="TextBox 31">
@@ -2761,7 +2796,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="32" name="TextBox 31">
@@ -3140,265 +3175,265 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABFF2E6-1E13-48EF-9BE3-D6C90C46BEC8}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.90625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="14" max="14" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8" ht="48.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>-2.1</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>2.8</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="24">
         <v>-1.9</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="24">
         <v>3.61</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="24">
         <v>1</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="24">
         <v>1</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="25">
         <v>-1.9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>-0.2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="22">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>0.8</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="22">
         <v>0.9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>0.4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="22">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="22">
         <v>-1</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>-2.4</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="22">
         <v>3.9</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>-1.2</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="23">
         <v>10.8</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="22" t="s">
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="23" t="s">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
-      <c r="B14" s="23" t="s">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="23" t="s">
+    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="23" t="s">
+    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="24" t="s">
+    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="15"/>
+      <c r="B17" s="18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3423,6 +3458,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ca1cba85-b018-40b2-9d9a-243cd5b6fae5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010070F75838E79B0E48B83E8E3F5479A3A2" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2b0c304636f8f537543cd13f583db9d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ca1cba85-b018-40b2-9d9a-243cd5b6fae5" xmlns:ns4="f1fb8133-dfcb-4ab3-83e1-bcafde3f766a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f089f22c5ce4e61126931f7622145b2" ns3:_="" ns4:_="">
     <xsd:import namespace="ca1cba85-b018-40b2-9d9a-243cd5b6fae5"/>
@@ -3617,14 +3660,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ca1cba85-b018-40b2-9d9a-243cd5b6fae5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C96E0334-A0AA-41B5-AE21-CAD1C9D10746}">
   <ds:schemaRefs>
@@ -3634,6 +3669,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5E1B631-90B0-4D19-A35E-F8DC8BE167A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f1fb8133-dfcb-4ab3-83e1-bcafde3f766a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="ca1cba85-b018-40b2-9d9a-243cd5b6fae5"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBDDC771-C014-4A48-9FCA-802C556EA1D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3650,21 +3702,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5E1B631-90B0-4D19-A35E-F8DC8BE167A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f1fb8133-dfcb-4ab3-83e1-bcafde3f766a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="ca1cba85-b018-40b2-9d9a-243cd5b6fae5"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>